<commit_message>
getting rid of debugger and puts statements
</commit_message>
<xml_diff>
--- a/calendars/calendar-base.xlsx
+++ b/calendars/calendar-base.xlsx
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3108,7 +3108,6 @@
     <hyperlink ref="D103" r:id="rId1" display="https://my.thoughtworks.com/docs/DOC-17202"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>